<commit_message>
Regretion and Fix SCD0174
</commit_message>
<xml_diff>
--- a/File_Upload/Template_upload_data_leads-2.xlsx
+++ b/File_Upload/Template_upload_data_leads-2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\File_Upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\File_Upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075B6AB6-4D41-463A-B0D8-D2F4D80F5EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95279613-71CC-494A-8B87-8DFDF2D73953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D23C01D4-F513-4B3F-82FB-F0F6A2A5DC95}"/>
   </bookViews>
@@ -131,25 +131,25 @@
     <t>082277268094</t>
   </si>
   <si>
-    <t>dedic 15</t>
-  </si>
-  <si>
-    <t>dedic 16</t>
-  </si>
-  <si>
-    <t>dedic 17</t>
-  </si>
-  <si>
-    <t>dedic 18</t>
-  </si>
-  <si>
-    <t>dedic 19</t>
-  </si>
-  <si>
-    <t>dedic 20</t>
-  </si>
-  <si>
-    <t>dedic 21</t>
+    <t>dedic 36</t>
+  </si>
+  <si>
+    <t>dedic 37</t>
+  </si>
+  <si>
+    <t>dedic 38</t>
+  </si>
+  <si>
+    <t>dedic 39</t>
+  </si>
+  <si>
+    <t>dedic 40</t>
+  </si>
+  <si>
+    <t>dedic 41</t>
+  </si>
+  <si>
+    <t>dedic 42</t>
   </si>
 </sst>
 </file>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A1360F-2012-4AFD-A638-BBBAA1DB64E1}">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +649,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>9020304177</v>
+        <v>9020304198</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -718,7 +718,8 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>9020304178</v>
+        <f>A2+1</f>
+        <v>9020304199</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -787,7 +788,8 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>9020304179</v>
+        <f t="shared" ref="A4:A8" si="1">A3+1</f>
+        <v>9020304200</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -847,7 +849,8 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>9020304180</v>
+        <f t="shared" si="1"/>
+        <v>9020304201</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
@@ -907,7 +910,8 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>9020304181</v>
+        <f t="shared" si="1"/>
+        <v>9020304202</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -967,7 +971,8 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>9020304182</v>
+        <f t="shared" si="1"/>
+        <v>9020304203</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
@@ -1033,7 +1038,8 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9020304183</v>
+        <f t="shared" si="1"/>
+        <v>9020304204</v>
       </c>
       <c r="B8" t="s">
         <v>38</v>

</xml_diff>